<commit_message>
Slight modifications to the code to process realigned RNA-Seq data (hg37->hg38) and the new interaction data from CRAPome "filter only" adjustment. Minor bug fixes. As a consequnence most downstream result files (figures and tables) are also updated.
</commit_message>
<xml_diff>
--- a/Supplementary_Table_S1_all_significant_links_HHIP.xlsx
+++ b/Supplementary_Table_S1_all_significant_links_HHIP.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I115"/>
+  <dimension ref="A1:I110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,29 +543,29 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>EIF2S2</t>
+          <t>TUBB4B</t>
         </is>
       </c>
       <c r="C4" t="n">
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -574,7 +574,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>RPLP0</t>
+          <t>CALM1</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -590,13 +590,13 @@
         <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -605,11 +605,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>TFG</t>
+          <t>CAVIN1</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -621,13 +621,13 @@
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -636,14 +636,14 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>TUBB4B</t>
+          <t>TMED2</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
@@ -655,10 +655,10 @@
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -667,29 +667,29 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>THBS1</t>
+          <t>TMED10</t>
         </is>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -698,7 +698,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>CALM1</t>
+          <t>ASPH</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -717,10 +717,10 @@
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -729,14 +729,14 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>EIF2S3</t>
+          <t>MMP9</t>
         </is>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -748,7 +748,7 @@
         <v>1</v>
       </c>
       <c r="H10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" t="n">
         <v>2</v>
@@ -760,14 +760,14 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>HSPA5</t>
+          <t>CALR</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
@@ -791,7 +791,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>TMED2</t>
+          <t>GORASP2</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -822,20 +822,20 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>CALR</t>
+          <t>MAP4</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -853,7 +853,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>MAP4</t>
+          <t>HSPA5</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -863,10 +863,10 @@
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
@@ -884,20 +884,20 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>MARCKS</t>
+          <t>EIF2S2</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
@@ -915,7 +915,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>MMP9</t>
+          <t>THBS1</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -946,26 +946,26 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>GORASP2</t>
+          <t>RRBP1</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" t="n">
         <v>2</v>
@@ -977,20 +977,20 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ASPH</t>
+          <t>MARCKS</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
@@ -1008,7 +1008,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>CAVIN1</t>
+          <t>RPLP0</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -1039,7 +1039,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>HSPA1A</t>
+          <t>HMGN1</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -1049,13 +1049,13 @@
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" t="n">
         <v>1</v>
@@ -1070,26 +1070,26 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>RRBP1</t>
+          <t>TP53</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" t="n">
         <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" t="n">
         <v>2</v>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>TMED10</t>
+          <t>TMED7</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -1132,7 +1132,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>EIF2S1</t>
+          <t>GREM1</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -1145,10 +1145,10 @@
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
@@ -1163,7 +1163,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>HMGN1</t>
+          <t>TUBA1B</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -1182,10 +1182,10 @@
         <v>0</v>
       </c>
       <c r="H24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -1194,17 +1194,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>TP53</t>
+          <t>RPL24</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" t="n">
         <v>0</v>
@@ -1213,10 +1213,10 @@
         <v>0</v>
       </c>
       <c r="H25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -1225,17 +1225,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>TMED7</t>
+          <t>YBX1</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26" t="n">
         <v>0</v>
@@ -1244,10 +1244,10 @@
         <v>0</v>
       </c>
       <c r="H26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -1256,7 +1256,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>GREM1</t>
+          <t>RACK1</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -1269,7 +1269,7 @@
         <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G27" t="n">
         <v>0</v>
@@ -1278,7 +1278,7 @@
         <v>0</v>
       </c>
       <c r="I27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -1287,11 +1287,11 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>EEF1A1</t>
+          <t>IGF2BP3</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" t="n">
         <v>0</v>
@@ -1303,13 +1303,13 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -1318,7 +1318,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>RPL24</t>
+          <t>RPL10A</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -1349,14 +1349,14 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>RPL19</t>
+          <t>RPS21</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" t="n">
         <v>0</v>
@@ -1380,14 +1380,14 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>HNRNPU</t>
+          <t>SKP1</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
@@ -1411,17 +1411,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>TUBA1B</t>
+          <t>RPL8</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32" t="n">
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F32" t="n">
         <v>0</v>
@@ -1442,7 +1442,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>IGF2BP3</t>
+          <t>RPL11</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -1473,7 +1473,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>YBX1</t>
+          <t>HNRNPU</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -1504,7 +1504,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>RACK1</t>
+          <t>RPL31</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -1535,14 +1535,14 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>RPS21</t>
+          <t>RPS28</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
@@ -1566,14 +1566,14 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>SKP1</t>
+          <t>RPS26</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E37" t="n">
         <v>0</v>
@@ -1597,7 +1597,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>RPL6</t>
+          <t>RPS25</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1628,7 +1628,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>RPL11</t>
+          <t>RPS24</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -1659,7 +1659,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>RPL10A</t>
+          <t>RPS6</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -1690,7 +1690,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>RPL31</t>
+          <t>RPL19</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -1721,7 +1721,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>RPS28</t>
+          <t>MVP</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -1752,7 +1752,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>RPS26</t>
+          <t>RPL6</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -1783,7 +1783,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>RPS25</t>
+          <t>RPL18</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1814,14 +1814,14 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>RPL8</t>
+          <t>RUVBL1</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E45" t="n">
         <v>0</v>
@@ -1845,14 +1845,14 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>MAP7D1</t>
+          <t>RUVBL2</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46" t="n">
         <v>0</v>
@@ -1876,7 +1876,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>RPL18</t>
+          <t>G3BP2</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1907,7 +1907,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>CKAP4</t>
+          <t>IGF2BP1</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>RUVBL1</t>
+          <t>DDX21</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1969,14 +1969,14 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>RUVBL2</t>
+          <t>HNRNPUL1</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E50" t="n">
         <v>0</v>
@@ -2000,7 +2000,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>G3BP2</t>
+          <t>TUBB6</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -2031,7 +2031,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>IGF2BP1</t>
+          <t>TUBA1C</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -2062,7 +2062,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>DDX21</t>
+          <t>USP9X</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -2093,7 +2093,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>HNRNPUL1</t>
+          <t>DDX17</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -2124,14 +2124,14 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>TUBB6</t>
+          <t>ABCF1</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E55" t="n">
         <v>0</v>
@@ -2155,11 +2155,11 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>PYM1</t>
+          <t>MAP7D1</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D56" t="n">
         <v>0</v>
@@ -2171,7 +2171,7 @@
         <v>0</v>
       </c>
       <c r="G56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H56" t="n">
         <v>0</v>
@@ -2186,7 +2186,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>TUBA1C</t>
+          <t>RPS4X</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -2217,7 +2217,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>USP9X</t>
+          <t>SF3B2</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -2248,17 +2248,17 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>DDX17</t>
+          <t>AHNAK</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D59" t="n">
         <v>0</v>
       </c>
       <c r="E59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F59" t="n">
         <v>0</v>
@@ -2279,14 +2279,14 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>ABCF1</t>
+          <t>DHX9</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E60" t="n">
         <v>0</v>
@@ -2310,7 +2310,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>RPS6</t>
+          <t>CKAP4</t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -2341,7 +2341,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>MVP</t>
+          <t>RPL23A</t>
         </is>
       </c>
       <c r="C62" t="n">
@@ -2372,14 +2372,14 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>SF3B2</t>
+          <t>RPS8</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E63" t="n">
         <v>0</v>
@@ -2403,17 +2403,17 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>AHNAK</t>
+          <t>RPL7A</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D64" t="n">
         <v>0</v>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F64" t="n">
         <v>0</v>
@@ -2434,7 +2434,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>DHX9</t>
+          <t>H1-5</t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -2465,14 +2465,14 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>RPS24</t>
+          <t>PTBP1</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E66" t="n">
         <v>0</v>
@@ -2496,7 +2496,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>RPS15A</t>
+          <t>RPL13</t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -2527,14 +2527,14 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>RPL23A</t>
+          <t>ATP5F1A</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E68" t="n">
         <v>0</v>
@@ -2558,7 +2558,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>RPS4X</t>
+          <t>RPS3</t>
         </is>
       </c>
       <c r="C69" t="n">
@@ -2589,14 +2589,14 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>CAD</t>
+          <t>NCL</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E70" t="n">
         <v>0</v>
@@ -2620,7 +2620,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>RPL10</t>
+          <t>RPL17</t>
         </is>
       </c>
       <c r="C71" t="n">
@@ -2651,14 +2651,14 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>PTBP1</t>
+          <t>RPL7</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D72" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E72" t="n">
         <v>0</v>
@@ -2682,7 +2682,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>RPL13</t>
+          <t>DDX5</t>
         </is>
       </c>
       <c r="C73" t="n">
@@ -2713,14 +2713,14 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>ATP5F1A</t>
+          <t>H1-3</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D74" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E74" t="n">
         <v>0</v>
@@ -2744,17 +2744,17 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>RPS3</t>
+          <t>HSP90B1</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D75" t="n">
         <v>0</v>
       </c>
       <c r="E75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F75" t="n">
         <v>0</v>
@@ -2775,14 +2775,14 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>NCL</t>
+          <t>CAD</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E76" t="n">
         <v>0</v>
@@ -2806,7 +2806,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>RPL17</t>
+          <t>XRCC5</t>
         </is>
       </c>
       <c r="C77" t="n">
@@ -2837,7 +2837,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>RPL7</t>
+          <t>HSPA8</t>
         </is>
       </c>
       <c r="C78" t="n">
@@ -2868,14 +2868,14 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>DDX5</t>
+          <t>HSPD1</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E79" t="n">
         <v>0</v>
@@ -2899,7 +2899,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>H1-3</t>
+          <t>HNRNPA1</t>
         </is>
       </c>
       <c r="C80" t="n">
@@ -2930,7 +2930,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>H1-5</t>
+          <t>TUBB</t>
         </is>
       </c>
       <c r="C81" t="n">
@@ -2961,17 +2961,17 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>HSP90B1</t>
+          <t>NPM1</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D82" t="n">
         <v>0</v>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F82" t="n">
         <v>0</v>
@@ -2992,7 +2992,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>XRCC5</t>
+          <t>RPLP2</t>
         </is>
       </c>
       <c r="C83" t="n">
@@ -3023,7 +3023,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>HSPA8</t>
+          <t>EIF2S1</t>
         </is>
       </c>
       <c r="C84" t="n">
@@ -3054,7 +3054,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>HSPD1</t>
+          <t>EIF5B</t>
         </is>
       </c>
       <c r="C85" t="n">
@@ -3085,7 +3085,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>HNRNPA1</t>
+          <t>RPL10</t>
         </is>
       </c>
       <c r="C86" t="n">
@@ -3116,17 +3116,17 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>TUBB</t>
+          <t>CANX</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D87" t="n">
         <v>0</v>
       </c>
       <c r="E87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>0</v>
@@ -3147,7 +3147,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>NPM1</t>
+          <t>RPS18</t>
         </is>
       </c>
       <c r="C88" t="n">
@@ -3178,7 +3178,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>RPLP2</t>
+          <t>ACTB</t>
         </is>
       </c>
       <c r="C89" t="n">
@@ -3209,14 +3209,14 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>EIF5B</t>
+          <t>RPS23</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D90" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E90" t="n">
         <v>0</v>
@@ -3240,17 +3240,17 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>CANX</t>
+          <t>RPS14</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D91" t="n">
         <v>0</v>
       </c>
       <c r="E91" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F91" t="n">
         <v>0</v>
@@ -3271,17 +3271,17 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>PDIA3</t>
+          <t>RPS16</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D92" t="n">
         <v>0</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F92" t="n">
         <v>0</v>
@@ -3302,14 +3302,14 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>NMT1</t>
+          <t>RPS15A</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D93" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E93" t="n">
         <v>0</v>
@@ -3333,7 +3333,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>RPS3A</t>
+          <t>SYNCRIP</t>
         </is>
       </c>
       <c r="C94" t="n">
@@ -3364,7 +3364,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>RPL7A</t>
+          <t>RPL15</t>
         </is>
       </c>
       <c r="C95" t="n">
@@ -3395,7 +3395,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>RPS18</t>
+          <t>RPL26</t>
         </is>
       </c>
       <c r="C96" t="n">
@@ -3426,7 +3426,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>RPS23</t>
+          <t>RPS3A</t>
         </is>
       </c>
       <c r="C97" t="n">
@@ -3457,7 +3457,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>RPS14</t>
+          <t>RPS20</t>
         </is>
       </c>
       <c r="C98" t="n">
@@ -3488,7 +3488,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>RPS16</t>
+          <t>HNRNPM</t>
         </is>
       </c>
       <c r="C99" t="n">
@@ -3519,17 +3519,17 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>SYNCRIP</t>
+          <t>PDIA3</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D100" t="n">
         <v>0</v>
       </c>
       <c r="E100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F100" t="n">
         <v>0</v>
@@ -3550,7 +3550,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>RPS8</t>
+          <t>HNRNPA3</t>
         </is>
       </c>
       <c r="C101" t="n">
@@ -3581,7 +3581,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>RPL15</t>
+          <t>RPS9</t>
         </is>
       </c>
       <c r="C102" t="n">
@@ -3612,14 +3612,14 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>RPL26</t>
+          <t>RPL5</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D103" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E103" t="n">
         <v>0</v>
@@ -3643,7 +3643,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>RPS20</t>
+          <t>RPL3</t>
         </is>
       </c>
       <c r="C104" t="n">
@@ -3674,7 +3674,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>HNRNPH1</t>
+          <t>RBMX</t>
         </is>
       </c>
       <c r="C105" t="n">
@@ -3705,7 +3705,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>ACTB</t>
+          <t>RPL4</t>
         </is>
       </c>
       <c r="C106" t="n">
@@ -3736,14 +3736,14 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>HNRNPM</t>
+          <t>CTNNA1</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D107" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E107" t="n">
         <v>0</v>
@@ -3767,7 +3767,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>HNRNPA3</t>
+          <t>HNRNPH1</t>
         </is>
       </c>
       <c r="C108" t="n">
@@ -3798,14 +3798,14 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>RPS9</t>
+          <t>NMT1</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D109" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E109" t="n">
         <v>0</v>
@@ -3829,14 +3829,14 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>RPL5</t>
+          <t>IGF2BP2</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D110" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E110" t="n">
         <v>0</v>
@@ -3851,161 +3851,6 @@
         <v>0</v>
       </c>
       <c r="I110" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" s="1" t="n">
-        <v>109</v>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>RPL3</t>
-        </is>
-      </c>
-      <c r="C111" t="n">
-        <v>1</v>
-      </c>
-      <c r="D111" t="n">
-        <v>0</v>
-      </c>
-      <c r="E111" t="n">
-        <v>0</v>
-      </c>
-      <c r="F111" t="n">
-        <v>0</v>
-      </c>
-      <c r="G111" t="n">
-        <v>0</v>
-      </c>
-      <c r="H111" t="n">
-        <v>0</v>
-      </c>
-      <c r="I111" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" s="1" t="n">
-        <v>110</v>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>RBMX</t>
-        </is>
-      </c>
-      <c r="C112" t="n">
-        <v>1</v>
-      </c>
-      <c r="D112" t="n">
-        <v>0</v>
-      </c>
-      <c r="E112" t="n">
-        <v>0</v>
-      </c>
-      <c r="F112" t="n">
-        <v>0</v>
-      </c>
-      <c r="G112" t="n">
-        <v>0</v>
-      </c>
-      <c r="H112" t="n">
-        <v>0</v>
-      </c>
-      <c r="I112" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" s="1" t="n">
-        <v>111</v>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>RPL4</t>
-        </is>
-      </c>
-      <c r="C113" t="n">
-        <v>1</v>
-      </c>
-      <c r="D113" t="n">
-        <v>0</v>
-      </c>
-      <c r="E113" t="n">
-        <v>0</v>
-      </c>
-      <c r="F113" t="n">
-        <v>0</v>
-      </c>
-      <c r="G113" t="n">
-        <v>0</v>
-      </c>
-      <c r="H113" t="n">
-        <v>0</v>
-      </c>
-      <c r="I113" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" s="1" t="n">
-        <v>112</v>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>CTNNA1</t>
-        </is>
-      </c>
-      <c r="C114" t="n">
-        <v>0</v>
-      </c>
-      <c r="D114" t="n">
-        <v>1</v>
-      </c>
-      <c r="E114" t="n">
-        <v>0</v>
-      </c>
-      <c r="F114" t="n">
-        <v>0</v>
-      </c>
-      <c r="G114" t="n">
-        <v>0</v>
-      </c>
-      <c r="H114" t="n">
-        <v>0</v>
-      </c>
-      <c r="I114" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" s="1" t="n">
-        <v>113</v>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>IGF2BP2</t>
-        </is>
-      </c>
-      <c r="C115" t="n">
-        <v>1</v>
-      </c>
-      <c r="D115" t="n">
-        <v>0</v>
-      </c>
-      <c r="E115" t="n">
-        <v>0</v>
-      </c>
-      <c r="F115" t="n">
-        <v>0</v>
-      </c>
-      <c r="G115" t="n">
-        <v>0</v>
-      </c>
-      <c r="H115" t="n">
-        <v>0</v>
-      </c>
-      <c r="I115" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>